<commit_message>
Updating vocab for keyword extraction (ontology data)
</commit_message>
<xml_diff>
--- a/vocab_updated.xlsx
+++ b/vocab_updated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\MSc\Code\MScProject\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1485B3B8-6A88-49F8-81EB-6100525562FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67492428-1A7B-4EDB-861D-E781CC86EC39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="235">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1678" uniqueCount="234">
   <si>
     <t>tag</t>
   </si>
@@ -631,18 +631,12 @@
     <t>Updated spelling</t>
   </si>
   <si>
-    <t>specific to Austrian market (where the exp was conducted)</t>
-  </si>
-  <si>
     <t>Not English word (mostly German)</t>
   </si>
   <si>
     <t>Made it bi-gram</t>
   </si>
   <si>
-    <t>specific to Estonian market (where the exp was conducted)</t>
-  </si>
-  <si>
     <t>free from lactose</t>
   </si>
   <si>
@@ -685,9 +679,6 @@
     <t>climate friendly</t>
   </si>
   <si>
-    <t>specific to exp conducted</t>
-  </si>
-  <si>
     <t>fresh product</t>
   </si>
   <si>
@@ -725,6 +716,12 @@
   </si>
   <si>
     <t>No Change</t>
+  </si>
+  <si>
+    <t>Specific to Estonian market (where the exp was conducted)</t>
+  </si>
+  <si>
+    <t>Specific to exp conducted</t>
   </si>
 </sst>
 </file>
@@ -1095,7 +1092,7 @@
   <dimension ref="A1:H335"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H329" sqref="H329"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1159,7 +1156,7 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -1185,7 +1182,7 @@
         <v>0</v>
       </c>
       <c r="H3" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.35">
@@ -1211,7 +1208,7 @@
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.35">
@@ -1237,7 +1234,7 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -1263,7 +1260,7 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
@@ -1289,7 +1286,7 @@
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.35">
@@ -1315,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="H8" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.35">
@@ -1341,7 +1338,7 @@
         <v>0</v>
       </c>
       <c r="H9" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.35">
@@ -1367,7 +1364,7 @@
         <v>0</v>
       </c>
       <c r="H10" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -1393,7 +1390,7 @@
         <v>0</v>
       </c>
       <c r="H11" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
@@ -1419,7 +1416,7 @@
         <v>0</v>
       </c>
       <c r="H12" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
@@ -1445,7 +1442,7 @@
         <v>0</v>
       </c>
       <c r="H13" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
@@ -1471,7 +1468,7 @@
         <v>0</v>
       </c>
       <c r="H14" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
@@ -1497,7 +1494,7 @@
         <v>0</v>
       </c>
       <c r="H15" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.35">
@@ -1523,7 +1520,7 @@
         <v>0</v>
       </c>
       <c r="H16" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.35">
@@ -1549,7 +1546,7 @@
         <v>0</v>
       </c>
       <c r="H17" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.35">
@@ -1575,7 +1572,7 @@
         <v>0</v>
       </c>
       <c r="H18" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.35">
@@ -1601,7 +1598,7 @@
         <v>0</v>
       </c>
       <c r="H19" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.35">
@@ -1627,7 +1624,7 @@
         <v>0</v>
       </c>
       <c r="H20" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.35">
@@ -1653,7 +1650,7 @@
         <v>0</v>
       </c>
       <c r="H21" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.35">
@@ -1679,7 +1676,7 @@
         <v>0</v>
       </c>
       <c r="H22" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.35">
@@ -1705,7 +1702,7 @@
         <v>0</v>
       </c>
       <c r="H23" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.35">
@@ -1757,7 +1754,7 @@
         <v>0</v>
       </c>
       <c r="H25" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.35">
@@ -1783,7 +1780,7 @@
         <v>0</v>
       </c>
       <c r="H26" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.35">
@@ -1806,10 +1803,10 @@
         <v>176</v>
       </c>
       <c r="G27">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H27" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.35">
@@ -1832,10 +1829,10 @@
         <v>176</v>
       </c>
       <c r="G28">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H28" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.35">
@@ -1858,10 +1855,10 @@
         <v>176</v>
       </c>
       <c r="G29">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H29" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.35">
@@ -1884,10 +1881,10 @@
         <v>176</v>
       </c>
       <c r="G30">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H30" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.35">
@@ -1910,10 +1907,10 @@
         <v>176</v>
       </c>
       <c r="G31">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H31" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.35">
@@ -1936,10 +1933,10 @@
         <v>176</v>
       </c>
       <c r="G32">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H32" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.35">
@@ -1962,10 +1959,10 @@
         <v>176</v>
       </c>
       <c r="G33">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H33" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.35">
@@ -1988,10 +1985,10 @@
         <v>176</v>
       </c>
       <c r="G34">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H34" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.35">
@@ -2014,10 +2011,10 @@
         <v>176</v>
       </c>
       <c r="G35">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H35" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.35">
@@ -2040,10 +2037,10 @@
         <v>176</v>
       </c>
       <c r="G36">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H36" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.35">
@@ -2066,10 +2063,10 @@
         <v>176</v>
       </c>
       <c r="G37">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H37" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.35">
@@ -2092,10 +2089,10 @@
         <v>176</v>
       </c>
       <c r="G38">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H38" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.35">
@@ -2118,10 +2115,10 @@
         <v>176</v>
       </c>
       <c r="G39">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H39" t="s">
-        <v>203</v>
+        <v>231</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.35">
@@ -2147,7 +2144,7 @@
         <v>-1</v>
       </c>
       <c r="H40" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.35">
@@ -2173,7 +2170,7 @@
         <v>0</v>
       </c>
       <c r="H41" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.35">
@@ -2199,7 +2196,7 @@
         <v>0</v>
       </c>
       <c r="H42" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.35">
@@ -2225,7 +2222,7 @@
         <v>0</v>
       </c>
       <c r="H43" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.35">
@@ -2251,7 +2248,7 @@
         <v>0</v>
       </c>
       <c r="H44" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.35">
@@ -2277,7 +2274,7 @@
         <v>0</v>
       </c>
       <c r="H45" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
@@ -2303,7 +2300,7 @@
         <v>0</v>
       </c>
       <c r="H46" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.35">
@@ -2329,7 +2326,7 @@
         <v>2</v>
       </c>
       <c r="H47" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.35">
@@ -2355,7 +2352,7 @@
         <v>0</v>
       </c>
       <c r="H48" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
@@ -2381,7 +2378,7 @@
         <v>0</v>
       </c>
       <c r="H49" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
@@ -2407,7 +2404,7 @@
         <v>0</v>
       </c>
       <c r="H50" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="51" spans="1:8" x14ac:dyDescent="0.35">
@@ -2433,7 +2430,7 @@
         <v>0</v>
       </c>
       <c r="H51" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="52" spans="1:8" x14ac:dyDescent="0.35">
@@ -2459,7 +2456,7 @@
         <v>0</v>
       </c>
       <c r="H52" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="53" spans="1:8" x14ac:dyDescent="0.35">
@@ -2485,7 +2482,7 @@
         <v>-1</v>
       </c>
       <c r="H53" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="54" spans="1:8" x14ac:dyDescent="0.35">
@@ -2511,7 +2508,7 @@
         <v>-1</v>
       </c>
       <c r="H54" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="55" spans="1:8" x14ac:dyDescent="0.35">
@@ -2537,7 +2534,7 @@
         <v>0</v>
       </c>
       <c r="H55" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="56" spans="1:8" x14ac:dyDescent="0.35">
@@ -2563,7 +2560,7 @@
         <v>0</v>
       </c>
       <c r="H56" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="57" spans="1:8" x14ac:dyDescent="0.35">
@@ -2589,7 +2586,7 @@
         <v>0</v>
       </c>
       <c r="H57" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="58" spans="1:8" x14ac:dyDescent="0.35">
@@ -2615,7 +2612,7 @@
         <v>0</v>
       </c>
       <c r="H58" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="59" spans="1:8" x14ac:dyDescent="0.35">
@@ -2641,7 +2638,7 @@
         <v>0</v>
       </c>
       <c r="H59" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="60" spans="1:8" x14ac:dyDescent="0.35">
@@ -2667,7 +2664,7 @@
         <v>0</v>
       </c>
       <c r="H60" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="61" spans="1:8" x14ac:dyDescent="0.35">
@@ -2693,7 +2690,7 @@
         <v>0</v>
       </c>
       <c r="H61" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="62" spans="1:8" x14ac:dyDescent="0.35">
@@ -2719,7 +2716,7 @@
         <v>0</v>
       </c>
       <c r="H62" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="63" spans="1:8" x14ac:dyDescent="0.35">
@@ -2745,7 +2742,7 @@
         <v>0</v>
       </c>
       <c r="H63" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="64" spans="1:8" x14ac:dyDescent="0.35">
@@ -2771,7 +2768,7 @@
         <v>0</v>
       </c>
       <c r="H64" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="65" spans="1:8" x14ac:dyDescent="0.35">
@@ -2797,7 +2794,7 @@
         <v>0</v>
       </c>
       <c r="H65" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="66" spans="1:8" x14ac:dyDescent="0.35">
@@ -2823,7 +2820,7 @@
         <v>0</v>
       </c>
       <c r="H66" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="67" spans="1:8" x14ac:dyDescent="0.35">
@@ -2849,7 +2846,7 @@
         <v>0</v>
       </c>
       <c r="H67" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.35">
@@ -2875,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="H68" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.35">
@@ -2901,7 +2898,7 @@
         <v>0</v>
       </c>
       <c r="H69" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.35">
@@ -2927,7 +2924,7 @@
         <v>0</v>
       </c>
       <c r="H70" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.35">
@@ -2953,7 +2950,7 @@
         <v>0</v>
       </c>
       <c r="H71" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.35">
@@ -2979,7 +2976,7 @@
         <v>0</v>
       </c>
       <c r="H72" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="73" spans="1:8" x14ac:dyDescent="0.35">
@@ -3005,7 +3002,7 @@
         <v>0</v>
       </c>
       <c r="H73" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="74" spans="1:8" x14ac:dyDescent="0.35">
@@ -3031,7 +3028,7 @@
         <v>0</v>
       </c>
       <c r="H74" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -3057,7 +3054,7 @@
         <v>0</v>
       </c>
       <c r="H75" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.35">
@@ -3083,7 +3080,7 @@
         <v>0</v>
       </c>
       <c r="H76" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.35">
@@ -3109,7 +3106,7 @@
         <v>0</v>
       </c>
       <c r="H77" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.35">
@@ -3135,7 +3132,7 @@
         <v>0</v>
       </c>
       <c r="H78" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.35">
@@ -3161,7 +3158,7 @@
         <v>0</v>
       </c>
       <c r="H79" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:8" x14ac:dyDescent="0.35">
@@ -3187,7 +3184,7 @@
         <v>0</v>
       </c>
       <c r="H80" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.35">
@@ -3213,7 +3210,7 @@
         <v>0</v>
       </c>
       <c r="H81" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.35">
@@ -3239,7 +3236,7 @@
         <v>0</v>
       </c>
       <c r="H82" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.35">
@@ -3265,7 +3262,7 @@
         <v>0</v>
       </c>
       <c r="H83" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.35">
@@ -3291,7 +3288,7 @@
         <v>0</v>
       </c>
       <c r="H84" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.35">
@@ -3317,7 +3314,7 @@
         <v>0</v>
       </c>
       <c r="H85" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="86" spans="1:8" x14ac:dyDescent="0.35">
@@ -3343,7 +3340,7 @@
         <v>0</v>
       </c>
       <c r="H86" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="87" spans="1:8" x14ac:dyDescent="0.35">
@@ -3369,7 +3366,7 @@
         <v>0</v>
       </c>
       <c r="H87" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="88" spans="1:8" x14ac:dyDescent="0.35">
@@ -3395,7 +3392,7 @@
         <v>0</v>
       </c>
       <c r="H88" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="89" spans="1:8" x14ac:dyDescent="0.35">
@@ -3421,7 +3418,7 @@
         <v>0</v>
       </c>
       <c r="H89" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.35">
@@ -3447,7 +3444,7 @@
         <v>0</v>
       </c>
       <c r="H90" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.35">
@@ -3473,7 +3470,7 @@
         <v>0</v>
       </c>
       <c r="H91" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.35">
@@ -3499,7 +3496,7 @@
         <v>0</v>
       </c>
       <c r="H92" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.35">
@@ -3525,7 +3522,7 @@
         <v>0</v>
       </c>
       <c r="H93" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="94" spans="1:8" x14ac:dyDescent="0.35">
@@ -3551,7 +3548,7 @@
         <v>0</v>
       </c>
       <c r="H94" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="95" spans="1:8" x14ac:dyDescent="0.35">
@@ -3577,7 +3574,7 @@
         <v>0</v>
       </c>
       <c r="H95" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="96" spans="1:8" x14ac:dyDescent="0.35">
@@ -3603,7 +3600,7 @@
         <v>0</v>
       </c>
       <c r="H96" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="97" spans="1:8" x14ac:dyDescent="0.35">
@@ -3629,7 +3626,7 @@
         <v>0</v>
       </c>
       <c r="H97" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="98" spans="1:8" x14ac:dyDescent="0.35">
@@ -3655,7 +3652,7 @@
         <v>0</v>
       </c>
       <c r="H98" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="99" spans="1:8" x14ac:dyDescent="0.35">
@@ -3681,7 +3678,7 @@
         <v>0</v>
       </c>
       <c r="H99" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="100" spans="1:8" x14ac:dyDescent="0.35">
@@ -3707,7 +3704,7 @@
         <v>0</v>
       </c>
       <c r="H100" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="101" spans="1:8" x14ac:dyDescent="0.35">
@@ -3733,7 +3730,7 @@
         <v>0</v>
       </c>
       <c r="H101" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="102" spans="1:8" x14ac:dyDescent="0.35">
@@ -3759,7 +3756,7 @@
         <v>0</v>
       </c>
       <c r="H102" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="103" spans="1:8" x14ac:dyDescent="0.35">
@@ -3785,7 +3782,7 @@
         <v>0</v>
       </c>
       <c r="H103" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="104" spans="1:8" x14ac:dyDescent="0.35">
@@ -3811,7 +3808,7 @@
         <v>0</v>
       </c>
       <c r="H104" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="105" spans="1:8" x14ac:dyDescent="0.35">
@@ -3837,7 +3834,7 @@
         <v>0</v>
       </c>
       <c r="H105" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="106" spans="1:8" x14ac:dyDescent="0.35">
@@ -3863,7 +3860,7 @@
         <v>0</v>
       </c>
       <c r="H106" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="107" spans="1:8" x14ac:dyDescent="0.35">
@@ -3889,7 +3886,7 @@
         <v>0</v>
       </c>
       <c r="H107" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="108" spans="1:8" x14ac:dyDescent="0.35">
@@ -3915,7 +3912,7 @@
         <v>0</v>
       </c>
       <c r="H108" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="109" spans="1:8" x14ac:dyDescent="0.35">
@@ -3941,7 +3938,7 @@
         <v>0</v>
       </c>
       <c r="H109" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="110" spans="1:8" x14ac:dyDescent="0.35">
@@ -3967,7 +3964,7 @@
         <v>0</v>
       </c>
       <c r="H110" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="111" spans="1:8" x14ac:dyDescent="0.35">
@@ -3993,7 +3990,7 @@
         <v>0</v>
       </c>
       <c r="H111" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="112" spans="1:8" x14ac:dyDescent="0.35">
@@ -4019,7 +4016,7 @@
         <v>0</v>
       </c>
       <c r="H112" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="113" spans="1:8" x14ac:dyDescent="0.35">
@@ -4045,7 +4042,7 @@
         <v>0</v>
       </c>
       <c r="H113" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="114" spans="1:8" x14ac:dyDescent="0.35">
@@ -4071,7 +4068,7 @@
         <v>0</v>
       </c>
       <c r="H114" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="115" spans="1:8" x14ac:dyDescent="0.35">
@@ -4097,7 +4094,7 @@
         <v>0</v>
       </c>
       <c r="H115" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="116" spans="1:8" x14ac:dyDescent="0.35">
@@ -4123,7 +4120,7 @@
         <v>0</v>
       </c>
       <c r="H116" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="117" spans="1:8" x14ac:dyDescent="0.35">
@@ -4146,10 +4143,10 @@
         <v>176</v>
       </c>
       <c r="G117">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H117" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="118" spans="1:8" x14ac:dyDescent="0.35">
@@ -4172,10 +4169,10 @@
         <v>176</v>
       </c>
       <c r="G118">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H118" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="119" spans="1:8" x14ac:dyDescent="0.35">
@@ -4198,10 +4195,10 @@
         <v>176</v>
       </c>
       <c r="G119">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H119" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="120" spans="1:8" x14ac:dyDescent="0.35">
@@ -4224,10 +4221,10 @@
         <v>176</v>
       </c>
       <c r="G120">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H120" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="121" spans="1:8" x14ac:dyDescent="0.35">
@@ -4250,10 +4247,10 @@
         <v>176</v>
       </c>
       <c r="G121">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H121" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="122" spans="1:8" x14ac:dyDescent="0.35">
@@ -4276,10 +4273,10 @@
         <v>176</v>
       </c>
       <c r="G122">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H122" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="123" spans="1:8" x14ac:dyDescent="0.35">
@@ -4302,10 +4299,10 @@
         <v>176</v>
       </c>
       <c r="G123">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H123" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="124" spans="1:8" x14ac:dyDescent="0.35">
@@ -4328,10 +4325,10 @@
         <v>176</v>
       </c>
       <c r="G124">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H124" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="125" spans="1:8" x14ac:dyDescent="0.35">
@@ -4354,10 +4351,10 @@
         <v>176</v>
       </c>
       <c r="G125">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H125" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="126" spans="1:8" x14ac:dyDescent="0.35">
@@ -4380,10 +4377,10 @@
         <v>176</v>
       </c>
       <c r="G126">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H126" t="s">
-        <v>206</v>
+        <v>231</v>
       </c>
     </row>
     <row r="127" spans="1:8" x14ac:dyDescent="0.35">
@@ -4409,7 +4406,7 @@
         <v>-1</v>
       </c>
       <c r="H127" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="128" spans="1:8" x14ac:dyDescent="0.35">
@@ -4435,7 +4432,7 @@
         <v>0</v>
       </c>
       <c r="H128" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="129" spans="1:8" x14ac:dyDescent="0.35">
@@ -4461,7 +4458,7 @@
         <v>0</v>
       </c>
       <c r="H129" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="130" spans="1:8" x14ac:dyDescent="0.35">
@@ -4487,7 +4484,7 @@
         <v>0</v>
       </c>
       <c r="H130" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="131" spans="1:8" x14ac:dyDescent="0.35">
@@ -4513,7 +4510,7 @@
         <v>0</v>
       </c>
       <c r="H131" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="132" spans="1:8" x14ac:dyDescent="0.35">
@@ -4539,7 +4536,7 @@
         <v>0</v>
       </c>
       <c r="H132" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="133" spans="1:8" x14ac:dyDescent="0.35">
@@ -4565,7 +4562,7 @@
         <v>0</v>
       </c>
       <c r="H133" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="134" spans="1:8" x14ac:dyDescent="0.35">
@@ -4591,7 +4588,7 @@
         <v>0</v>
       </c>
       <c r="H134" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="135" spans="1:8" x14ac:dyDescent="0.35">
@@ -4617,7 +4614,7 @@
         <v>0</v>
       </c>
       <c r="H135" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="136" spans="1:8" x14ac:dyDescent="0.35">
@@ -4643,7 +4640,7 @@
         <v>0</v>
       </c>
       <c r="H136" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="137" spans="1:8" x14ac:dyDescent="0.35">
@@ -4669,7 +4666,7 @@
         <v>0</v>
       </c>
       <c r="H137" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="138" spans="1:8" x14ac:dyDescent="0.35">
@@ -4695,7 +4692,7 @@
         <v>0</v>
       </c>
       <c r="H138" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="139" spans="1:8" x14ac:dyDescent="0.35">
@@ -4721,7 +4718,7 @@
         <v>0</v>
       </c>
       <c r="H139" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="140" spans="1:8" x14ac:dyDescent="0.35">
@@ -4747,7 +4744,7 @@
         <v>0</v>
       </c>
       <c r="H140" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="141" spans="1:8" x14ac:dyDescent="0.35">
@@ -4773,7 +4770,7 @@
         <v>0</v>
       </c>
       <c r="H141" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="142" spans="1:8" x14ac:dyDescent="0.35">
@@ -4799,7 +4796,7 @@
         <v>0</v>
       </c>
       <c r="H142" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="143" spans="1:8" x14ac:dyDescent="0.35">
@@ -4825,7 +4822,7 @@
         <v>0</v>
       </c>
       <c r="H143" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="144" spans="1:8" x14ac:dyDescent="0.35">
@@ -4851,7 +4848,7 @@
         <v>0</v>
       </c>
       <c r="H144" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="145" spans="1:8" x14ac:dyDescent="0.35">
@@ -4877,7 +4874,7 @@
         <v>0</v>
       </c>
       <c r="H145" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="146" spans="1:8" x14ac:dyDescent="0.35">
@@ -4903,7 +4900,7 @@
         <v>0</v>
       </c>
       <c r="H146" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="147" spans="1:8" x14ac:dyDescent="0.35">
@@ -4929,7 +4926,7 @@
         <v>0</v>
       </c>
       <c r="H147" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="148" spans="1:8" x14ac:dyDescent="0.35">
@@ -4955,7 +4952,7 @@
         <v>0</v>
       </c>
       <c r="H148" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="149" spans="1:8" x14ac:dyDescent="0.35">
@@ -4981,7 +4978,7 @@
         <v>0</v>
       </c>
       <c r="H149" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="150" spans="1:8" x14ac:dyDescent="0.35">
@@ -5007,7 +5004,7 @@
         <v>0</v>
       </c>
       <c r="H150" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="151" spans="1:8" x14ac:dyDescent="0.35">
@@ -5033,7 +5030,7 @@
         <v>0</v>
       </c>
       <c r="H151" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="152" spans="1:8" x14ac:dyDescent="0.35">
@@ -5059,7 +5056,7 @@
         <v>0</v>
       </c>
       <c r="H152" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="153" spans="1:8" x14ac:dyDescent="0.35">
@@ -5085,7 +5082,7 @@
         <v>0</v>
       </c>
       <c r="H153" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="154" spans="1:8" x14ac:dyDescent="0.35">
@@ -5111,7 +5108,7 @@
         <v>-1</v>
       </c>
       <c r="H154" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="155" spans="1:8" x14ac:dyDescent="0.35">
@@ -5137,7 +5134,7 @@
         <v>0</v>
       </c>
       <c r="H155" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="156" spans="1:8" x14ac:dyDescent="0.35">
@@ -5163,7 +5160,7 @@
         <v>0</v>
       </c>
       <c r="H156" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="157" spans="1:8" x14ac:dyDescent="0.35">
@@ -5189,7 +5186,7 @@
         <v>-1</v>
       </c>
       <c r="H157" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="158" spans="1:8" x14ac:dyDescent="0.35">
@@ -5215,7 +5212,7 @@
         <v>0</v>
       </c>
       <c r="H158" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="159" spans="1:8" x14ac:dyDescent="0.35">
@@ -5241,7 +5238,7 @@
         <v>0</v>
       </c>
       <c r="H159" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="160" spans="1:8" x14ac:dyDescent="0.35">
@@ -5267,7 +5264,7 @@
         <v>0</v>
       </c>
       <c r="H160" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="161" spans="1:8" x14ac:dyDescent="0.35">
@@ -5293,7 +5290,7 @@
         <v>0</v>
       </c>
       <c r="H161" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="162" spans="1:8" x14ac:dyDescent="0.35">
@@ -5319,7 +5316,7 @@
         <v>-1</v>
       </c>
       <c r="H162" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
     </row>
     <row r="163" spans="1:8" x14ac:dyDescent="0.35">
@@ -5345,7 +5342,7 @@
         <v>-1</v>
       </c>
       <c r="H163" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
     </row>
     <row r="164" spans="1:8" x14ac:dyDescent="0.35">
@@ -5371,7 +5368,7 @@
         <v>-1</v>
       </c>
       <c r="H164" t="s">
-        <v>206</v>
+        <v>232</v>
       </c>
     </row>
     <row r="165" spans="1:8" x14ac:dyDescent="0.35">
@@ -5397,7 +5394,7 @@
         <v>0</v>
       </c>
       <c r="H165" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="166" spans="1:8" x14ac:dyDescent="0.35">
@@ -5423,7 +5420,7 @@
         <v>0</v>
       </c>
       <c r="H166" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="167" spans="1:8" x14ac:dyDescent="0.35">
@@ -5449,7 +5446,7 @@
         <v>0</v>
       </c>
       <c r="H167" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="168" spans="1:8" x14ac:dyDescent="0.35">
@@ -5475,7 +5472,7 @@
         <v>0</v>
       </c>
       <c r="H168" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="169" spans="1:8" x14ac:dyDescent="0.35">
@@ -5501,7 +5498,7 @@
         <v>0</v>
       </c>
       <c r="H169" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="170" spans="1:8" x14ac:dyDescent="0.35">
@@ -5527,7 +5524,7 @@
         <v>0</v>
       </c>
       <c r="H170" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="171" spans="1:8" x14ac:dyDescent="0.35">
@@ -5553,7 +5550,7 @@
         <v>0</v>
       </c>
       <c r="H171" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="172" spans="1:8" x14ac:dyDescent="0.35">
@@ -5579,7 +5576,7 @@
         <v>0</v>
       </c>
       <c r="H172" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="173" spans="1:8" x14ac:dyDescent="0.35">
@@ -5605,7 +5602,7 @@
         <v>0</v>
       </c>
       <c r="H173" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="174" spans="1:8" x14ac:dyDescent="0.35">
@@ -5631,7 +5628,7 @@
         <v>0</v>
       </c>
       <c r="H174" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="175" spans="1:8" x14ac:dyDescent="0.35">
@@ -5657,7 +5654,7 @@
         <v>0</v>
       </c>
       <c r="H175" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:8" x14ac:dyDescent="0.35">
@@ -5683,7 +5680,7 @@
         <v>0</v>
       </c>
       <c r="H176" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="177" spans="1:8" x14ac:dyDescent="0.35">
@@ -5709,7 +5706,7 @@
         <v>0</v>
       </c>
       <c r="H177" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="178" spans="1:8" x14ac:dyDescent="0.35">
@@ -5735,7 +5732,7 @@
         <v>0</v>
       </c>
       <c r="H178" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="179" spans="1:8" x14ac:dyDescent="0.35">
@@ -5761,7 +5758,7 @@
         <v>0</v>
       </c>
       <c r="H179" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="180" spans="1:8" x14ac:dyDescent="0.35">
@@ -5787,7 +5784,7 @@
         <v>0</v>
       </c>
       <c r="H180" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="181" spans="1:8" x14ac:dyDescent="0.35">
@@ -5813,7 +5810,7 @@
         <v>0</v>
       </c>
       <c r="H181" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="182" spans="1:8" x14ac:dyDescent="0.35">
@@ -5839,7 +5836,7 @@
         <v>0</v>
       </c>
       <c r="H182" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="183" spans="1:8" x14ac:dyDescent="0.35">
@@ -5865,7 +5862,7 @@
         <v>0</v>
       </c>
       <c r="H183" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="184" spans="1:8" x14ac:dyDescent="0.35">
@@ -5891,7 +5888,7 @@
         <v>0</v>
       </c>
       <c r="H184" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="185" spans="1:8" x14ac:dyDescent="0.35">
@@ -5917,7 +5914,7 @@
         <v>0</v>
       </c>
       <c r="H185" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="186" spans="1:8" x14ac:dyDescent="0.35">
@@ -5943,7 +5940,7 @@
         <v>0</v>
       </c>
       <c r="H186" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="187" spans="1:8" x14ac:dyDescent="0.35">
@@ -5951,7 +5948,7 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="C187" t="s">
         <v>162</v>
@@ -5995,7 +5992,7 @@
         <v>0</v>
       </c>
       <c r="H188" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="189" spans="1:8" x14ac:dyDescent="0.35">
@@ -6021,7 +6018,7 @@
         <v>0</v>
       </c>
       <c r="H189" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="190" spans="1:8" x14ac:dyDescent="0.35">
@@ -6047,7 +6044,7 @@
         <v>0</v>
       </c>
       <c r="H190" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="191" spans="1:8" x14ac:dyDescent="0.35">
@@ -6073,7 +6070,7 @@
         <v>0</v>
       </c>
       <c r="H191" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="192" spans="1:8" x14ac:dyDescent="0.35">
@@ -6099,7 +6096,7 @@
         <v>0</v>
       </c>
       <c r="H192" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="193" spans="1:8" x14ac:dyDescent="0.35">
@@ -6125,7 +6122,7 @@
         <v>0</v>
       </c>
       <c r="H193" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="194" spans="1:8" x14ac:dyDescent="0.35">
@@ -6133,7 +6130,7 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C194" t="s">
         <v>166</v>
@@ -6151,7 +6148,7 @@
         <v>2</v>
       </c>
       <c r="H194" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="195" spans="1:8" x14ac:dyDescent="0.35">
@@ -6177,7 +6174,7 @@
         <v>0</v>
       </c>
       <c r="H195" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="196" spans="1:8" x14ac:dyDescent="0.35">
@@ -6203,7 +6200,7 @@
         <v>0</v>
       </c>
       <c r="H196" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="197" spans="1:8" x14ac:dyDescent="0.35">
@@ -6229,7 +6226,7 @@
         <v>0</v>
       </c>
       <c r="H197" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="198" spans="1:8" x14ac:dyDescent="0.35">
@@ -6255,7 +6252,7 @@
         <v>0</v>
       </c>
       <c r="H198" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="199" spans="1:8" x14ac:dyDescent="0.35">
@@ -6281,7 +6278,7 @@
         <v>0</v>
       </c>
       <c r="H199" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="200" spans="1:8" x14ac:dyDescent="0.35">
@@ -6307,7 +6304,7 @@
         <v>0</v>
       </c>
       <c r="H200" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="201" spans="1:8" x14ac:dyDescent="0.35">
@@ -6333,7 +6330,7 @@
         <v>0</v>
       </c>
       <c r="H201" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="202" spans="1:8" x14ac:dyDescent="0.35">
@@ -6359,7 +6356,7 @@
         <v>0</v>
       </c>
       <c r="H202" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="203" spans="1:8" x14ac:dyDescent="0.35">
@@ -6385,7 +6382,7 @@
         <v>0</v>
       </c>
       <c r="H203" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="204" spans="1:8" x14ac:dyDescent="0.35">
@@ -6411,7 +6408,7 @@
         <v>0</v>
       </c>
       <c r="H204" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="205" spans="1:8" x14ac:dyDescent="0.35">
@@ -6437,7 +6434,7 @@
         <v>0</v>
       </c>
       <c r="H205" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="206" spans="1:8" x14ac:dyDescent="0.35">
@@ -6463,7 +6460,7 @@
         <v>0</v>
       </c>
       <c r="H206" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="207" spans="1:8" x14ac:dyDescent="0.35">
@@ -6489,7 +6486,7 @@
         <v>0</v>
       </c>
       <c r="H207" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="208" spans="1:8" x14ac:dyDescent="0.35">
@@ -6515,7 +6512,7 @@
         <v>0</v>
       </c>
       <c r="H208" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="209" spans="1:8" x14ac:dyDescent="0.35">
@@ -6541,7 +6538,7 @@
         <v>0</v>
       </c>
       <c r="H209" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="210" spans="1:8" x14ac:dyDescent="0.35">
@@ -6567,7 +6564,7 @@
         <v>0</v>
       </c>
       <c r="H210" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="211" spans="1:8" x14ac:dyDescent="0.35">
@@ -6593,7 +6590,7 @@
         <v>0</v>
       </c>
       <c r="H211" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="212" spans="1:8" x14ac:dyDescent="0.35">
@@ -6619,7 +6616,7 @@
         <v>0</v>
       </c>
       <c r="H212" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="213" spans="1:8" x14ac:dyDescent="0.35">
@@ -6645,7 +6642,7 @@
         <v>0</v>
       </c>
       <c r="H213" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="214" spans="1:8" x14ac:dyDescent="0.35">
@@ -6671,7 +6668,7 @@
         <v>0</v>
       </c>
       <c r="H214" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="215" spans="1:8" x14ac:dyDescent="0.35">
@@ -6697,7 +6694,7 @@
         <v>0</v>
       </c>
       <c r="H215" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="216" spans="1:8" x14ac:dyDescent="0.35">
@@ -6723,7 +6720,7 @@
         <v>0</v>
       </c>
       <c r="H216" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="217" spans="1:8" x14ac:dyDescent="0.35">
@@ -6749,7 +6746,7 @@
         <v>0</v>
       </c>
       <c r="H217" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="218" spans="1:8" x14ac:dyDescent="0.35">
@@ -6775,7 +6772,7 @@
         <v>0</v>
       </c>
       <c r="H218" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="219" spans="1:8" x14ac:dyDescent="0.35">
@@ -6801,7 +6798,7 @@
         <v>0</v>
       </c>
       <c r="H219" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="220" spans="1:8" x14ac:dyDescent="0.35">
@@ -6827,7 +6824,7 @@
         <v>0</v>
       </c>
       <c r="H220" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="221" spans="1:8" x14ac:dyDescent="0.35">
@@ -6853,7 +6850,7 @@
         <v>0</v>
       </c>
       <c r="H221" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="222" spans="1:8" x14ac:dyDescent="0.35">
@@ -6879,7 +6876,7 @@
         <v>0</v>
       </c>
       <c r="H222" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="223" spans="1:8" x14ac:dyDescent="0.35">
@@ -6905,7 +6902,7 @@
         <v>0</v>
       </c>
       <c r="H223" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="224" spans="1:8" x14ac:dyDescent="0.35">
@@ -6931,7 +6928,7 @@
         <v>0</v>
       </c>
       <c r="H224" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="225" spans="1:8" x14ac:dyDescent="0.35">
@@ -6957,7 +6954,7 @@
         <v>0</v>
       </c>
       <c r="H225" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="226" spans="1:8" x14ac:dyDescent="0.35">
@@ -6983,7 +6980,7 @@
         <v>0</v>
       </c>
       <c r="H226" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="227" spans="1:8" x14ac:dyDescent="0.35">
@@ -7009,7 +7006,7 @@
         <v>0</v>
       </c>
       <c r="H227" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="228" spans="1:8" x14ac:dyDescent="0.35">
@@ -7035,7 +7032,7 @@
         <v>0</v>
       </c>
       <c r="H228" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="229" spans="1:8" x14ac:dyDescent="0.35">
@@ -7061,7 +7058,7 @@
         <v>0</v>
       </c>
       <c r="H229" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="230" spans="1:8" x14ac:dyDescent="0.35">
@@ -7087,7 +7084,7 @@
         <v>0</v>
       </c>
       <c r="H230" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="231" spans="1:8" x14ac:dyDescent="0.35">
@@ -7113,7 +7110,7 @@
         <v>0</v>
       </c>
       <c r="H231" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="232" spans="1:8" x14ac:dyDescent="0.35">
@@ -7139,7 +7136,7 @@
         <v>0</v>
       </c>
       <c r="H232" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="233" spans="1:8" x14ac:dyDescent="0.35">
@@ -7165,7 +7162,7 @@
         <v>0</v>
       </c>
       <c r="H233" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="234" spans="1:8" x14ac:dyDescent="0.35">
@@ -7191,7 +7188,7 @@
         <v>0</v>
       </c>
       <c r="H234" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="235" spans="1:8" x14ac:dyDescent="0.35">
@@ -7217,7 +7214,7 @@
         <v>0</v>
       </c>
       <c r="H235" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="236" spans="1:8" x14ac:dyDescent="0.35">
@@ -7243,7 +7240,7 @@
         <v>0</v>
       </c>
       <c r="H236" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="237" spans="1:8" x14ac:dyDescent="0.35">
@@ -7251,7 +7248,7 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="C237" t="s">
         <v>154</v>
@@ -7269,7 +7266,7 @@
         <v>2</v>
       </c>
       <c r="H237" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="238" spans="1:8" x14ac:dyDescent="0.35">
@@ -7295,7 +7292,7 @@
         <v>0</v>
       </c>
       <c r="H238" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="239" spans="1:8" x14ac:dyDescent="0.35">
@@ -7321,7 +7318,7 @@
         <v>0</v>
       </c>
       <c r="H239" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="240" spans="1:8" x14ac:dyDescent="0.35">
@@ -7347,7 +7344,7 @@
         <v>0</v>
       </c>
       <c r="H240" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="241" spans="1:8" x14ac:dyDescent="0.35">
@@ -7355,7 +7352,7 @@
         <v>239</v>
       </c>
       <c r="B241" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="C241" t="s">
         <v>156</v>
@@ -7373,7 +7370,7 @@
         <v>2</v>
       </c>
       <c r="H241" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="242" spans="1:8" x14ac:dyDescent="0.35">
@@ -7399,7 +7396,7 @@
         <v>0</v>
       </c>
       <c r="H242" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="243" spans="1:8" x14ac:dyDescent="0.35">
@@ -7425,7 +7422,7 @@
         <v>0</v>
       </c>
       <c r="H243" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="244" spans="1:8" x14ac:dyDescent="0.35">
@@ -7451,7 +7448,7 @@
         <v>-1</v>
       </c>
       <c r="H244" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
     </row>
     <row r="245" spans="1:8" x14ac:dyDescent="0.35">
@@ -7474,10 +7471,10 @@
         <v>1</v>
       </c>
       <c r="G245">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="H245" t="s">
-        <v>221</v>
+        <v>231</v>
       </c>
     </row>
     <row r="246" spans="1:8" x14ac:dyDescent="0.35">
@@ -7503,7 +7500,7 @@
         <v>0</v>
       </c>
       <c r="H246" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="247" spans="1:8" x14ac:dyDescent="0.35">
@@ -7529,7 +7526,7 @@
         <v>0</v>
       </c>
       <c r="H247" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="248" spans="1:8" x14ac:dyDescent="0.35">
@@ -7555,7 +7552,7 @@
         <v>0</v>
       </c>
       <c r="H248" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="249" spans="1:8" x14ac:dyDescent="0.35">
@@ -7581,7 +7578,7 @@
         <v>0</v>
       </c>
       <c r="H249" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="250" spans="1:8" x14ac:dyDescent="0.35">
@@ -7607,7 +7604,7 @@
         <v>0</v>
       </c>
       <c r="H250" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="251" spans="1:8" x14ac:dyDescent="0.35">
@@ -7615,7 +7612,7 @@
         <v>249</v>
       </c>
       <c r="B251" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="C251" t="s">
         <v>167</v>
@@ -7633,7 +7630,7 @@
         <v>2</v>
       </c>
       <c r="H251" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="252" spans="1:8" x14ac:dyDescent="0.35">
@@ -7659,7 +7656,7 @@
         <v>0</v>
       </c>
       <c r="H252" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="253" spans="1:8" x14ac:dyDescent="0.35">
@@ -7685,7 +7682,7 @@
         <v>0</v>
       </c>
       <c r="H253" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="254" spans="1:8" x14ac:dyDescent="0.35">
@@ -7711,7 +7708,7 @@
         <v>0</v>
       </c>
       <c r="H254" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="255" spans="1:8" x14ac:dyDescent="0.35">
@@ -7737,7 +7734,7 @@
         <v>0</v>
       </c>
       <c r="H255" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="256" spans="1:8" x14ac:dyDescent="0.35">
@@ -7763,7 +7760,7 @@
         <v>0</v>
       </c>
       <c r="H256" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="257" spans="1:8" x14ac:dyDescent="0.35">
@@ -7789,7 +7786,7 @@
         <v>0</v>
       </c>
       <c r="H257" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="258" spans="1:8" x14ac:dyDescent="0.35">
@@ -7815,7 +7812,7 @@
         <v>0</v>
       </c>
       <c r="H258" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="259" spans="1:8" x14ac:dyDescent="0.35">
@@ -7841,7 +7838,7 @@
         <v>0</v>
       </c>
       <c r="H259" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="260" spans="1:8" x14ac:dyDescent="0.35">
@@ -7867,7 +7864,7 @@
         <v>0</v>
       </c>
       <c r="H260" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="261" spans="1:8" x14ac:dyDescent="0.35">
@@ -7893,7 +7890,7 @@
         <v>0</v>
       </c>
       <c r="H261" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="262" spans="1:8" x14ac:dyDescent="0.35">
@@ -7919,7 +7916,7 @@
         <v>0</v>
       </c>
       <c r="H262" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="263" spans="1:8" x14ac:dyDescent="0.35">
@@ -7945,7 +7942,7 @@
         <v>0</v>
       </c>
       <c r="H263" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="264" spans="1:8" x14ac:dyDescent="0.35">
@@ -7953,7 +7950,7 @@
         <v>262</v>
       </c>
       <c r="B264" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="C264" t="s">
         <v>157</v>
@@ -7997,7 +7994,7 @@
         <v>0</v>
       </c>
       <c r="H265" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="266" spans="1:8" x14ac:dyDescent="0.35">
@@ -8023,7 +8020,7 @@
         <v>0</v>
       </c>
       <c r="H266" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="267" spans="1:8" x14ac:dyDescent="0.35">
@@ -8049,7 +8046,7 @@
         <v>0</v>
       </c>
       <c r="H267" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="268" spans="1:8" x14ac:dyDescent="0.35">
@@ -8075,7 +8072,7 @@
         <v>0</v>
       </c>
       <c r="H268" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="269" spans="1:8" x14ac:dyDescent="0.35">
@@ -8101,7 +8098,7 @@
         <v>0</v>
       </c>
       <c r="H269" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="270" spans="1:8" x14ac:dyDescent="0.35">
@@ -8127,7 +8124,7 @@
         <v>0</v>
       </c>
       <c r="H270" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="271" spans="1:8" x14ac:dyDescent="0.35">
@@ -8153,7 +8150,7 @@
         <v>0</v>
       </c>
       <c r="H271" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="272" spans="1:8" x14ac:dyDescent="0.35">
@@ -8179,7 +8176,7 @@
         <v>-1</v>
       </c>
       <c r="H272" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="273" spans="1:8" x14ac:dyDescent="0.35">
@@ -8205,7 +8202,7 @@
         <v>-1</v>
       </c>
       <c r="H273" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="274" spans="1:8" x14ac:dyDescent="0.35">
@@ -8231,7 +8228,7 @@
         <v>-1</v>
       </c>
       <c r="H274" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="275" spans="1:8" x14ac:dyDescent="0.35">
@@ -8257,7 +8254,7 @@
         <v>0</v>
       </c>
       <c r="H275" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="276" spans="1:8" x14ac:dyDescent="0.35">
@@ -8283,7 +8280,7 @@
         <v>0</v>
       </c>
       <c r="H276" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="277" spans="1:8" x14ac:dyDescent="0.35">
@@ -8309,7 +8306,7 @@
         <v>0</v>
       </c>
       <c r="H277" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="278" spans="1:8" x14ac:dyDescent="0.35">
@@ -8335,7 +8332,7 @@
         <v>0</v>
       </c>
       <c r="H278" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="279" spans="1:8" x14ac:dyDescent="0.35">
@@ -8361,7 +8358,7 @@
         <v>0</v>
       </c>
       <c r="H279" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="280" spans="1:8" x14ac:dyDescent="0.35">
@@ -8387,7 +8384,7 @@
         <v>0</v>
       </c>
       <c r="H280" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="281" spans="1:8" x14ac:dyDescent="0.35">
@@ -8413,7 +8410,7 @@
         <v>0</v>
       </c>
       <c r="H281" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="282" spans="1:8" x14ac:dyDescent="0.35">
@@ -8439,7 +8436,7 @@
         <v>0</v>
       </c>
       <c r="H282" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="283" spans="1:8" x14ac:dyDescent="0.35">
@@ -8465,7 +8462,7 @@
         <v>0</v>
       </c>
       <c r="H283" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="284" spans="1:8" x14ac:dyDescent="0.35">
@@ -8491,7 +8488,7 @@
         <v>0</v>
       </c>
       <c r="H284" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="285" spans="1:8" x14ac:dyDescent="0.35">
@@ -8517,7 +8514,7 @@
         <v>0</v>
       </c>
       <c r="H285" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="286" spans="1:8" x14ac:dyDescent="0.35">
@@ -8543,7 +8540,7 @@
         <v>0</v>
       </c>
       <c r="H286" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="287" spans="1:8" x14ac:dyDescent="0.35">
@@ -8569,7 +8566,7 @@
         <v>0</v>
       </c>
       <c r="H287" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="288" spans="1:8" x14ac:dyDescent="0.35">
@@ -8595,7 +8592,7 @@
         <v>0</v>
       </c>
       <c r="H288" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="289" spans="1:8" x14ac:dyDescent="0.35">
@@ -8621,7 +8618,7 @@
         <v>0</v>
       </c>
       <c r="H289" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="290" spans="1:8" x14ac:dyDescent="0.35">
@@ -8647,7 +8644,7 @@
         <v>0</v>
       </c>
       <c r="H290" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="291" spans="1:8" x14ac:dyDescent="0.35">
@@ -8673,7 +8670,7 @@
         <v>0</v>
       </c>
       <c r="H291" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="292" spans="1:8" x14ac:dyDescent="0.35">
@@ -8699,7 +8696,7 @@
         <v>0</v>
       </c>
       <c r="H292" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="293" spans="1:8" x14ac:dyDescent="0.35">
@@ -8725,7 +8722,7 @@
         <v>0</v>
       </c>
       <c r="H293" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="294" spans="1:8" x14ac:dyDescent="0.35">
@@ -8751,7 +8748,7 @@
         <v>0</v>
       </c>
       <c r="H294" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="295" spans="1:8" x14ac:dyDescent="0.35">
@@ -8777,7 +8774,7 @@
         <v>0</v>
       </c>
       <c r="H295" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="296" spans="1:8" x14ac:dyDescent="0.35">
@@ -8803,7 +8800,7 @@
         <v>0</v>
       </c>
       <c r="H296" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="297" spans="1:8" x14ac:dyDescent="0.35">
@@ -8829,7 +8826,7 @@
         <v>0</v>
       </c>
       <c r="H297" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="298" spans="1:8" x14ac:dyDescent="0.35">
@@ -8855,7 +8852,7 @@
         <v>0</v>
       </c>
       <c r="H298" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="299" spans="1:8" x14ac:dyDescent="0.35">
@@ -8881,7 +8878,7 @@
         <v>0</v>
       </c>
       <c r="H299" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="300" spans="1:8" x14ac:dyDescent="0.35">
@@ -8907,7 +8904,7 @@
         <v>1</v>
       </c>
       <c r="H300" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="301" spans="1:8" x14ac:dyDescent="0.35">
@@ -8933,7 +8930,7 @@
         <v>1</v>
       </c>
       <c r="H301" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="302" spans="1:8" x14ac:dyDescent="0.35">
@@ -8959,7 +8956,7 @@
         <v>1</v>
       </c>
       <c r="H302" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="303" spans="1:8" x14ac:dyDescent="0.35">
@@ -8985,7 +8982,7 @@
         <v>1</v>
       </c>
       <c r="H303" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="304" spans="1:8" x14ac:dyDescent="0.35">
@@ -9011,7 +9008,7 @@
         <v>1</v>
       </c>
       <c r="H304" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="305" spans="1:8" x14ac:dyDescent="0.35">
@@ -9037,7 +9034,7 @@
         <v>1</v>
       </c>
       <c r="H305" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="306" spans="1:8" x14ac:dyDescent="0.35">
@@ -9063,7 +9060,7 @@
         <v>1</v>
       </c>
       <c r="H306" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="307" spans="1:8" x14ac:dyDescent="0.35">
@@ -9089,7 +9086,7 @@
         <v>1</v>
       </c>
       <c r="H307" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="308" spans="1:8" x14ac:dyDescent="0.35">
@@ -9115,7 +9112,7 @@
         <v>1</v>
       </c>
       <c r="H308" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="309" spans="1:8" x14ac:dyDescent="0.35">
@@ -9141,7 +9138,7 @@
         <v>1</v>
       </c>
       <c r="H309" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="310" spans="1:8" x14ac:dyDescent="0.35">
@@ -9167,7 +9164,7 @@
         <v>1</v>
       </c>
       <c r="H310" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="311" spans="1:8" x14ac:dyDescent="0.35">
@@ -9193,7 +9190,7 @@
         <v>1</v>
       </c>
       <c r="H311" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="312" spans="1:8" x14ac:dyDescent="0.35">
@@ -9219,7 +9216,7 @@
         <v>1</v>
       </c>
       <c r="H312" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="313" spans="1:8" x14ac:dyDescent="0.35">
@@ -9245,7 +9242,7 @@
         <v>1</v>
       </c>
       <c r="H313" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="314" spans="1:8" x14ac:dyDescent="0.35">
@@ -9271,7 +9268,7 @@
         <v>1</v>
       </c>
       <c r="H314" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="315" spans="1:8" x14ac:dyDescent="0.35">
@@ -9297,7 +9294,7 @@
         <v>1</v>
       </c>
       <c r="H315" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="316" spans="1:8" x14ac:dyDescent="0.35">
@@ -9323,7 +9320,7 @@
         <v>1</v>
       </c>
       <c r="H316" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="317" spans="1:8" x14ac:dyDescent="0.35">
@@ -9349,7 +9346,7 @@
         <v>1</v>
       </c>
       <c r="H317" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="318" spans="1:8" x14ac:dyDescent="0.35">
@@ -9357,7 +9354,7 @@
         <v>153</v>
       </c>
       <c r="B318" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C318" t="s">
         <v>148</v>
@@ -9375,7 +9372,7 @@
         <v>1</v>
       </c>
       <c r="H318" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="319" spans="1:8" x14ac:dyDescent="0.35">
@@ -9383,7 +9380,7 @@
         <v>154</v>
       </c>
       <c r="B319" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="C319" t="s">
         <v>160</v>
@@ -9401,7 +9398,7 @@
         <v>1</v>
       </c>
       <c r="H319" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
     </row>
     <row r="320" spans="1:8" x14ac:dyDescent="0.35">
@@ -9427,7 +9424,7 @@
         <v>1</v>
       </c>
       <c r="H320" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="321" spans="1:8" x14ac:dyDescent="0.35">
@@ -9435,7 +9432,7 @@
         <v>192</v>
       </c>
       <c r="B321" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="C321" t="s">
         <v>166</v>
@@ -9453,7 +9450,7 @@
         <v>1</v>
       </c>
       <c r="H321" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
     </row>
     <row r="322" spans="1:8" x14ac:dyDescent="0.35">
@@ -9461,7 +9458,7 @@
         <v>216</v>
       </c>
       <c r="B322" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C322" t="s">
         <v>150</v>
@@ -9479,7 +9476,7 @@
         <v>1</v>
       </c>
       <c r="H322" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="323" spans="1:8" x14ac:dyDescent="0.35">
@@ -9487,7 +9484,7 @@
         <v>217</v>
       </c>
       <c r="B323" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C323" t="s">
         <v>159</v>
@@ -9505,7 +9502,7 @@
         <v>1</v>
       </c>
       <c r="H323" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="324" spans="1:8" x14ac:dyDescent="0.35">
@@ -9513,7 +9510,7 @@
         <v>218</v>
       </c>
       <c r="B324" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="C324" t="s">
         <v>151</v>
@@ -9531,7 +9528,7 @@
         <v>1</v>
       </c>
       <c r="H324" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="325" spans="1:8" x14ac:dyDescent="0.35">
@@ -9539,7 +9536,7 @@
         <v>216</v>
       </c>
       <c r="B325" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C325" t="s">
         <v>150</v>
@@ -9557,7 +9554,7 @@
         <v>1</v>
       </c>
       <c r="H325" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="326" spans="1:8" x14ac:dyDescent="0.35">
@@ -9565,7 +9562,7 @@
         <v>217</v>
       </c>
       <c r="B326" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C326" t="s">
         <v>159</v>
@@ -9583,7 +9580,7 @@
         <v>1</v>
       </c>
       <c r="H326" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="327" spans="1:8" x14ac:dyDescent="0.35">
@@ -9591,7 +9588,7 @@
         <v>218</v>
       </c>
       <c r="B327" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C327" t="s">
         <v>151</v>
@@ -9609,7 +9606,7 @@
         <v>1</v>
       </c>
       <c r="H327" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="328" spans="1:8" x14ac:dyDescent="0.35">
@@ -9617,7 +9614,7 @@
         <v>222</v>
       </c>
       <c r="B328" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C328" t="s">
         <v>159</v>
@@ -9635,7 +9632,7 @@
         <v>1</v>
       </c>
       <c r="H328" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="329" spans="1:8" x14ac:dyDescent="0.35">
@@ -9643,7 +9640,7 @@
         <v>222</v>
       </c>
       <c r="B329" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="C329" t="s">
         <v>159</v>
@@ -9661,7 +9658,7 @@
         <v>1</v>
       </c>
       <c r="H329" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="330" spans="1:8" x14ac:dyDescent="0.35">
@@ -9669,7 +9666,7 @@
         <v>236</v>
       </c>
       <c r="B330" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="C330" t="s">
         <v>153</v>
@@ -9687,7 +9684,7 @@
         <v>1</v>
       </c>
       <c r="H330" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="331" spans="1:8" x14ac:dyDescent="0.35">
@@ -9695,7 +9692,7 @@
         <v>236</v>
       </c>
       <c r="B331" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="C331" t="s">
         <v>153</v>
@@ -9713,7 +9710,7 @@
         <v>1</v>
       </c>
       <c r="H331" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="332" spans="1:8" x14ac:dyDescent="0.35">
@@ -9721,7 +9718,7 @@
         <v>265</v>
       </c>
       <c r="B332" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="C332" t="s">
         <v>153</v>
@@ -9739,7 +9736,7 @@
         <v>1</v>
       </c>
       <c r="H332" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="333" spans="1:8" x14ac:dyDescent="0.35">
@@ -9747,7 +9744,7 @@
         <v>265</v>
       </c>
       <c r="B333" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="C333" t="s">
         <v>153</v>
@@ -9765,7 +9762,7 @@
         <v>1</v>
       </c>
       <c r="H333" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="334" spans="1:8" x14ac:dyDescent="0.35">
@@ -9773,7 +9770,7 @@
         <v>265</v>
       </c>
       <c r="B334" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="C334" t="s">
         <v>153</v>
@@ -9791,7 +9788,7 @@
         <v>1</v>
       </c>
       <c r="H334" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
     </row>
     <row r="335" spans="1:8" x14ac:dyDescent="0.35">
@@ -9799,7 +9796,7 @@
         <v>266</v>
       </c>
       <c r="B335" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
       <c r="C335" t="s">
         <v>171</v>
@@ -9817,7 +9814,7 @@
         <v>1</v>
       </c>
       <c r="H335" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>